<commit_message>
Put col/row outline levels the right way around
</commit_message>
<xml_diff>
--- a/tests/testthat/outlines.xlsx
+++ b/tests/testthat/outlines.xlsx
@@ -32,6 +32,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -113,68 +114,68 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="B2:E5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="B1" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="C1" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="D1" s="0" t="n">
-        <v>14</v>
-      </c>
-    </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="B2" s="0" t="n">
         <v>21</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="C2" s="0" t="n">
         <v>22</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="D2" s="0" t="n">
         <v>23</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="E2" s="0" t="n">
         <v>24</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="B3" s="0" t="n">
         <v>31</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="C3" s="0" t="n">
         <v>32</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="D3" s="0" t="n">
         <v>33</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="E3" s="0" t="n">
         <v>34</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+      <c r="B4" s="0" t="n">
         <v>41</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="C4" s="0" t="n">
         <v>42</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="D4" s="0" t="n">
         <v>43</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="E4" s="0" t="n">
         <v>44</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="0" t="n">
+        <v>51</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>52</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>53</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -193,71 +194,71 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="B2:E5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.85"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="B1" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="C1" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="D1" s="0" t="n">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="0" t="n">
         <v>21</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="C2" s="0" t="n">
         <v>22</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="D2" s="0" t="n">
         <v>23</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="E2" s="0" t="n">
         <v>24</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+    <row r="3" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B3" s="0" t="n">
         <v>31</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="C3" s="0" t="n">
         <v>32</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="D3" s="0" t="n">
         <v>33</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="E3" s="0" t="n">
         <v>34</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+      <c r="B4" s="0" t="n">
         <v>41</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="C4" s="0" t="n">
         <v>42</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="D4" s="0" t="n">
         <v>43</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="E4" s="0" t="n">
         <v>44</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="0" t="n">
+        <v>51</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>52</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>53</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -276,73 +277,73 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="B2:E5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="3" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="3" outlineLevelCol="3"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="1" max="2" min="2" style="0" width="11.52"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="2" max="3" min="3" style="0" width="11.52"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="3" max="4" min="4" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="B1" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="C1" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="D1" s="0" t="n">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
-      <c r="A2" s="0" t="n">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="0" t="n">
         <v>21</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="C2" s="0" t="n">
         <v>22</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="D2" s="0" t="n">
         <v>23</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="E2" s="0" t="n">
         <v>24</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="2" collapsed="false">
-      <c r="A3" s="0" t="n">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+      <c r="B3" s="0" t="n">
         <v>31</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="C3" s="0" t="n">
         <v>32</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="D3" s="0" t="n">
         <v>33</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="E3" s="0" t="n">
         <v>34</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="3" collapsed="false">
-      <c r="A4" s="0" t="n">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="2" collapsed="false">
+      <c r="B4" s="0" t="n">
         <v>41</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="C4" s="0" t="n">
         <v>42</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="D4" s="0" t="n">
         <v>43</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="E4" s="0" t="n">
         <v>44</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="3" collapsed="false">
+      <c r="B5" s="0" t="n">
+        <v>51</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>52</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>53</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -361,13 +362,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="B1:E5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="3" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="3" outlineLevelCol="3"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.35"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="1" max="2" min="2" style="0" width="11.52"/>
@@ -375,60 +376,61 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="3" max="4" min="4" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="21.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="B1" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="C1" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="D1" s="0" t="n">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
-      <c r="A2" s="0" t="n">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="2" customFormat="false" ht="21.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B2" s="0" t="n">
         <v>21</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="C2" s="0" t="n">
         <v>22</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="D2" s="0" t="n">
         <v>23</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="E2" s="0" t="n">
         <v>24</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.9" hidden="false" customHeight="true" outlineLevel="2" collapsed="false">
-      <c r="A3" s="0" t="n">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+      <c r="B3" s="0" t="n">
         <v>31</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="C3" s="0" t="n">
         <v>32</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="D3" s="0" t="n">
         <v>33</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="E3" s="0" t="n">
         <v>34</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="3" collapsed="false">
-      <c r="A4" s="0" t="n">
+    <row r="4" customFormat="false" ht="15.9" hidden="false" customHeight="true" outlineLevel="2" collapsed="false">
+      <c r="B4" s="0" t="n">
         <v>41</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="C4" s="0" t="n">
         <v>42</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="D4" s="0" t="n">
         <v>43</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="E4" s="0" t="n">
         <v>44</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="3" collapsed="false">
+      <c r="B5" s="0" t="n">
+        <v>51</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>52</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>53</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>